<commit_message>
new change in code
</commit_message>
<xml_diff>
--- a/MyStoreProject/src/test/resources/TestData/TestData.xlsx
+++ b/MyStoreProject/src/test/resources/TestData/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15330" windowHeight="6615" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,10 @@
     <sheet name="ProductDetails" sheetId="4" r:id="rId4"/>
     <sheet name="SearchProduct" sheetId="6" r:id="rId5"/>
     <sheet name="AccountCreationData" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O20"/>
 </workbook>
 </file>
 
@@ -299,8 +301,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +465,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -541,6 +548,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -575,6 +583,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -750,14 +759,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
@@ -773,7 +782,7 @@
     <col min="13" max="13" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>44</v>
       </c>
@@ -781,7 +790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>42</v>
       </c>
@@ -789,7 +798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>43</v>
       </c>
@@ -797,7 +806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>38</v>
       </c>
@@ -806,7 +815,7 @@
       <c r="D4" s="14"/>
       <c r="E4" s="15"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -823,7 +832,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -840,7 +849,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -857,7 +866,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -874,7 +883,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -891,7 +900,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -908,7 +917,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -930,7 +939,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -945,7 +954,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
@@ -956,7 +965,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -965,7 +974,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -974,7 +983,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -983,7 +992,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1010,14 +1019,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
@@ -1026,7 +1035,7 @@
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>48</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>50</v>
       </c>
@@ -1053,22 +1062,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>58</v>
       </c>
@@ -1083,16 +1092,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>53</v>
       </c>
@@ -1103,7 +1112,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>56</v>
       </c>
@@ -1120,19 +1129,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>56</v>
       </c>
@@ -1143,14 +1152,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
@@ -1169,7 +1178,7 @@
     <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>52</v>
       </c>
@@ -1216,7 +1225,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>87</v>
       </c>
@@ -1263,7 +1272,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>88</v>
       </c>
@@ -1310,7 +1319,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>89</v>
       </c>
@@ -1365,4 +1374,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>